<commit_message>
Aggiunto excel per tutti i file di kruskal naive
</commit_message>
<xml_diff>
--- a/first assignment/result_prim.xlsx
+++ b/first assignment/result_prim.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davide/Sviluppo/Advanced Algorithm/first assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A3CA5B5D-441A-8847-AC5D-A0EA4975BDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95508DC8-CB87-BC49-A968-AB2AF8369C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="760" windowWidth="29200" windowHeight="18880"/>
+    <workbookView xWindow="260" yWindow="-19600" windowWidth="29200" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="result_prim" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -265,7 +262,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1799,161 +1796,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="result_kruskal_union_find"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="7">
-          <cell r="I7" t="str">
-            <v>Time (ms)</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="H8">
-            <v>10</v>
-          </cell>
-          <cell r="I8">
-            <v>1.8000000000000002E-2</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="H9">
-            <v>20</v>
-          </cell>
-          <cell r="I9">
-            <v>1.4477500000000001</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="H10">
-            <v>40</v>
-          </cell>
-          <cell r="I10">
-            <v>2.7499999999999997E-2</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="H11">
-            <v>80</v>
-          </cell>
-          <cell r="I11">
-            <v>6.275E-2</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="H12">
-            <v>100</v>
-          </cell>
-          <cell r="I12">
-            <v>6.7250000000000004E-2</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="H13">
-            <v>200</v>
-          </cell>
-          <cell r="I13">
-            <v>0.14725000000000002</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="H14">
-            <v>400</v>
-          </cell>
-          <cell r="I14">
-            <v>0.24875000000000003</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="H15">
-            <v>800</v>
-          </cell>
-          <cell r="I15">
-            <v>0.53500000000000003</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="H16">
-            <v>1000</v>
-          </cell>
-          <cell r="I16">
-            <v>0.77649999999999997</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="H17">
-            <v>2000</v>
-          </cell>
-          <cell r="I17">
-            <v>1.2362500000000001</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="H18">
-            <v>4000</v>
-          </cell>
-          <cell r="I18">
-            <v>3.1150000000000002</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="H19">
-            <v>8000</v>
-          </cell>
-          <cell r="I19">
-            <v>7.1852499999999999</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="H20">
-            <v>10000</v>
-          </cell>
-          <cell r="I20">
-            <v>10.257</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="H21">
-            <v>20000</v>
-          </cell>
-          <cell r="I21">
-            <v>18.333749999999998</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="H22">
-            <v>40000</v>
-          </cell>
-          <cell r="I22">
-            <v>32.538249999999998</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="H23">
-            <v>80000</v>
-          </cell>
-          <cell r="I23">
-            <v>96.396249999999995</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="H24">
-            <v>100000</v>
-          </cell>
-          <cell r="I24">
-            <v>110.66375000000001</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
@@ -2250,11 +2092,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>